<commit_message>
Added GENIE FORTRAN code (TOC + O2 working) + some boundary cond changes in tables + bullet points intro
</commit_message>
<xml_diff>
--- a/TeX/Diffusion_coefficients.xlsx
+++ b/TeX/Diffusion_coefficients.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>Parameters used to calculate diffusion coefficients</t>
   </si>
@@ -97,16 +97,17 @@
     <t>in Gypens language</t>
   </si>
   <si>
-    <t>Take </t>
+    <t>Take</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="0.00000" numFmtId="165"/>
+    <numFmt formatCode="0.000" numFmtId="166"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -278,13 +279,13 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
@@ -294,17 +295,19 @@
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="3" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="7" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="0" fontId="7" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="5" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="0" fontId="7" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="6" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="7" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="8" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="0" fontId="7" numFmtId="166" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="7" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="0" fontId="8" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
@@ -326,18 +329,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:N23"/>
+  <dimension ref="A3:N33"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="E15" activeCellId="0" pane="topLeft" sqref="E15"/>
+      <selection activeCell="F18" activeCellId="0" pane="topLeft" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5843137254902"/>
-    <col collapsed="false" hidden="false" max="9" min="4" style="0" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.7019607843137"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.6588235294118"/>
+    <col collapsed="false" hidden="false" max="9" min="4" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.7960784313725"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="3">
@@ -350,7 +353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="5">
       <c r="G5" s="2" t="s">
         <v>2</v>
       </c>
@@ -362,18 +365,18 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="J6" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="G7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.9" outlineLevel="0" r="8">
       <c r="A8" s="4"/>
       <c r="B8" s="5" t="s">
         <v>5</v>
@@ -385,7 +388,7 @@
         <v>7</v>
       </c>
       <c r="H8" s="0" t="n">
-        <f aca="false">+9.78*60*60/100^2</f>
+        <f aca="false">K10*60*60/100^2</f>
         <v>3.5208</v>
       </c>
       <c r="J8" s="4"/>
@@ -396,7 +399,7 @@
       <c r="M8" s="8"/>
       <c r="N8" s="9"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.9" outlineLevel="0" r="9">
       <c r="A9" s="10" t="s">
         <v>9</v>
       </c>
@@ -433,7 +436,7 @@
       </c>
       <c r="N9" s="14"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.9" outlineLevel="0" r="10">
       <c r="A10" s="10" t="s">
         <v>12</v>
       </c>
@@ -449,7 +452,7 @@
         <v>13</v>
       </c>
       <c r="H10" s="0" t="n">
-        <f aca="false">+5*60*60/100^2</f>
+        <f aca="false">K18*60*60/100^2</f>
         <v>1.8</v>
       </c>
       <c r="J10" s="13"/>
@@ -464,11 +467,11 @@
       </c>
       <c r="N10" s="14"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.9" outlineLevel="0" r="11">
       <c r="A11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="16" t="n">
+      <c r="B11" s="11" t="n">
         <f aca="false">3.5208*10^(-6)</f>
         <v>3.5208E-006</v>
       </c>
@@ -479,6 +482,10 @@
       <c r="G11" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="H11" s="16" t="n">
+        <f aca="false">K28*60*60/100^2</f>
+        <v>3.51</v>
+      </c>
       <c r="J11" s="13" t="s">
         <v>16</v>
       </c>
@@ -492,7 +499,7 @@
       </c>
       <c r="N11" s="14"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.9" outlineLevel="0" r="12">
       <c r="A12" s="10" t="s">
         <v>17</v>
       </c>
@@ -511,7 +518,7 @@
       </c>
       <c r="N12" s="14"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.9" outlineLevel="0" r="13">
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
@@ -540,7 +547,7 @@
         <v>0.149142857142857</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.9" outlineLevel="0" r="14">
       <c r="A14" s="10" t="s">
         <v>20</v>
       </c>
@@ -561,7 +568,7 @@
       <c r="M14" s="19"/>
       <c r="N14" s="20"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.9" outlineLevel="0" r="15">
       <c r="A15" s="10" t="s">
         <v>21</v>
       </c>
@@ -574,7 +581,7 @@
         <v>157.68</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.9" outlineLevel="0" r="16">
       <c r="A16" s="10" t="s">
         <v>22</v>
       </c>
@@ -594,11 +601,18 @@
       <c r="M16" s="8"/>
       <c r="N16" s="9"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="17">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.9" outlineLevel="0" r="17">
       <c r="A17" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="14"/>
+      <c r="B17" s="0" t="n">
+        <f aca="false">H11*10^(-6)</f>
+        <v>3.51E-006</v>
+      </c>
+      <c r="C17" s="21" t="n">
+        <f aca="false">+B17*24*365*100^2</f>
+        <v>307.476</v>
+      </c>
       <c r="J17" s="13" t="s">
         <v>11</v>
       </c>
@@ -613,12 +627,18 @@
       </c>
       <c r="N17" s="14"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="18">
-      <c r="A18" s="21" t="s">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.9" outlineLevel="0" r="18">
+      <c r="A18" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="20"/>
+      <c r="B18" s="23" t="n">
+        <f aca="false">K33*10^(-6)</f>
+        <v>1.1E-007</v>
+      </c>
+      <c r="C18" s="12" t="n">
+        <f aca="false">+B18*24*365*100^2</f>
+        <v>9.636</v>
+      </c>
       <c r="J18" s="13"/>
       <c r="K18" s="0" t="n">
         <v>5</v>
@@ -631,7 +651,7 @@
       </c>
       <c r="N18" s="14"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="J19" s="13" t="s">
         <v>16</v>
       </c>
@@ -645,7 +665,7 @@
       </c>
       <c r="N19" s="14"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="J20" s="13"/>
       <c r="M20" s="0" t="n">
         <f aca="false">(M18-L18)/(M17-L17)</f>
@@ -653,7 +673,7 @@
       </c>
       <c r="N20" s="14"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="J21" s="13" t="s">
         <v>25</v>
       </c>
@@ -671,7 +691,7 @@
         <v>0.0925714285714285</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22">
       <c r="J22" s="18"/>
       <c r="K22" s="19" t="n">
         <f aca="false">AVERAGE(M21:N21)</f>
@@ -681,12 +701,107 @@
       <c r="M22" s="19"/>
       <c r="N22" s="20"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="23">
-      <c r="J23" s="22" t="s">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="23">
+      <c r="J23" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="K23" s="23" t="n">
+      <c r="K23" s="25" t="n">
         <v>0.09</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="26">
+      <c r="J26" s="4"/>
+      <c r="K26" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="9"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
+      <c r="J27" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="M27" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="N27" s="14"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
+      <c r="J28" s="13"/>
+      <c r="K28" s="0" t="n">
+        <v>9.75</v>
+      </c>
+      <c r="L28" s="0" t="n">
+        <v>14.8</v>
+      </c>
+      <c r="M28" s="0" t="n">
+        <v>17.3</v>
+      </c>
+      <c r="N28" s="14"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
+      <c r="J29" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L29" s="0" t="n">
+        <f aca="false">(L28-K28)/18</f>
+        <v>0.280555555555556</v>
+      </c>
+      <c r="M29" s="0" t="n">
+        <f aca="false">(M28-K28)/25</f>
+        <v>0.302</v>
+      </c>
+      <c r="N29" s="14"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
+      <c r="J30" s="13"/>
+      <c r="M30" s="0" t="n">
+        <f aca="false">(M28-L28)/(M27-L27)</f>
+        <v>0.357142857142857</v>
+      </c>
+      <c r="N30" s="14"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
+      <c r="J31" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17" t="n">
+        <f aca="false">+L29*60^2/100^2</f>
+        <v>0.101</v>
+      </c>
+      <c r="M31" s="17" t="n">
+        <f aca="false">+M29*60^2/100^2</f>
+        <v>0.10872</v>
+      </c>
+      <c r="N31" s="14" t="n">
+        <f aca="false">+M30*60^2/100^2</f>
+        <v>0.128571428571429</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
+      <c r="J32" s="18"/>
+      <c r="K32" s="19" t="n">
+        <f aca="false">AVERAGE(M31:N31)</f>
+        <v>0.118645714285714</v>
+      </c>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="20"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="33">
+      <c r="J33" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="K33" s="25" t="n">
+        <v>0.11</v>
       </c>
     </row>
   </sheetData>
@@ -716,7 +831,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -741,7 +856,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
LaTeX: restructured cGENIE coupled reesults, now Invariant first...
</commit_message>
<xml_diff>
--- a/TeX/Diffusion_coefficients.xlsx
+++ b/TeX/Diffusion_coefficients.xlsx
@@ -8,8 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="185" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Diffcoeff" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Diff - advection" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="67">
   <si>
     <t>Schulz 2006</t>
   </si>
@@ -194,17 +194,42 @@
   </si>
   <si>
     <t>before I used NH4 value</t>
+  </si>
+  <si>
+    <t>SFD</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Depth of diagenesis where still affects SWI-fluxes</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>cm/yr</t>
+  </si>
+  <si>
+    <t>cm2/yr</t>
+  </si>
+  <si>
+    <t>cm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00E+000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -395,7 +420,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -537,6 +562,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -560,7 +593,7 @@
   <dimension ref="A2:AL42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R28" activeCellId="0" sqref="R28"/>
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2707,17 +2740,334 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="B3:E22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6887755102041"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C5" s="36" t="n">
+        <f aca="false"> 10^(-0.87478367-0.00043512*B5)*3.3</f>
+        <v>0.418768754094935</v>
+      </c>
+      <c r="D5" s="37" t="n">
+        <v>100</v>
+      </c>
+      <c r="E5" s="37" t="n">
+        <f aca="false">D5/C5</f>
+        <v>238.795275488319</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="C6" s="36" t="n">
+        <f aca="false"> 10^(-0.87478367-0.00043512*B6)*3.3</f>
+        <v>0.398307303520399</v>
+      </c>
+      <c r="D6" s="37" t="n">
+        <v>100</v>
+      </c>
+      <c r="E6" s="37" t="n">
+        <f aca="false">D6/C6</f>
+        <v>251.062431233774</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="C7" s="36" t="n">
+        <f aca="false"> 10^(-0.87478367-0.00043512*B7)*3.3</f>
+        <v>0.378845619417263</v>
+      </c>
+      <c r="D7" s="37" t="n">
+        <v>100</v>
+      </c>
+      <c r="E7" s="37" t="n">
+        <f aca="false">D7/C7</f>
+        <v>263.959763224448</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="C8" s="36" t="n">
+        <f aca="false"> 10^(-0.87478367-0.00043512*B8)*3.3</f>
+        <v>0.360334852218695</v>
+      </c>
+      <c r="D8" s="37" t="n">
+        <v>100</v>
+      </c>
+      <c r="E8" s="37" t="n">
+        <f aca="false">D8/C8</f>
+        <v>277.519644253861</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="C9" s="36" t="n">
+        <f aca="false"> 10^(-0.87478367-0.00043512*B9)*3.3</f>
+        <v>0.342728539195436</v>
+      </c>
+      <c r="D9" s="37" t="n">
+        <v>100</v>
+      </c>
+      <c r="E9" s="37" t="n">
+        <f aca="false">D9/C9</f>
+        <v>291.776110138807</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="C10" s="36" t="n">
+        <f aca="false"> 10^(-0.87478367-0.00043512*B10)*3.3</f>
+        <v>0.325982487832586</v>
+      </c>
+      <c r="D10" s="37" t="n">
+        <v>100</v>
+      </c>
+      <c r="E10" s="37" t="n">
+        <f aca="false">D10/C10</f>
+        <v>306.76494515054</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="n">
+        <v>350</v>
+      </c>
+      <c r="C11" s="36" t="n">
+        <f aca="false"> 10^(-0.87478367-0.00043512*B11)*3.3</f>
+        <v>0.310054664904712</v>
+      </c>
+      <c r="D11" s="37" t="n">
+        <v>100</v>
+      </c>
+      <c r="E11" s="37" t="n">
+        <f aca="false">D11/C11</f>
+        <v>322.523771834663</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="C12" s="36" t="n">
+        <f aca="false"> 10^(-0.87478367-0.00043512*B12)*3.3</f>
+        <v>0.294905090970851</v>
+      </c>
+      <c r="D12" s="37" t="n">
+        <v>100</v>
+      </c>
+      <c r="E12" s="37" t="n">
+        <f aca="false">D12/C12</f>
+        <v>339.09214544514</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="C13" s="36" t="n">
+        <f aca="false"> 10^(-0.87478367-0.00043512*B13)*3.3</f>
+        <v>0.266790444047381</v>
+      </c>
+      <c r="D13" s="37" t="n">
+        <v>100</v>
+      </c>
+      <c r="E13" s="37" t="n">
+        <f aca="false">D13/C13</f>
+        <v>374.826018814378</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C14" s="36" t="n">
+        <f aca="false"> 10^(-0.87478367-0.00043512*B14)*3.3</f>
+        <v>0.161662864535287</v>
+      </c>
+      <c r="D14" s="37" t="n">
+        <v>100</v>
+      </c>
+      <c r="E14" s="37" t="n">
+        <f aca="false">D14/C14</f>
+        <v>618.571248798902</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C15" s="36" t="n">
+        <f aca="false"> 10^(-0.87478367-0.00043512*B15)*3.3</f>
+        <v>0.0979603368594152</v>
+      </c>
+      <c r="D15" s="37" t="n">
+        <v>100</v>
+      </c>
+      <c r="E15" s="37" t="n">
+        <f aca="false">D15/C15</f>
+        <v>1020.82131611605</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C16" s="36" t="n">
+        <f aca="false"> 10^(-0.87478367-0.00043512*B16)*3.3</f>
+        <v>0.0593595048881217</v>
+      </c>
+      <c r="D16" s="37" t="n">
+        <v>100</v>
+      </c>
+      <c r="E16" s="37" t="n">
+        <f aca="false">D16/C16</f>
+        <v>1684.65016998501</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="n">
+        <v>2500</v>
+      </c>
+      <c r="C17" s="36" t="n">
+        <f aca="false"> 10^(-0.87478367-0.00043512*B17)*3.3</f>
+        <v>0.0359691578604886</v>
+      </c>
+      <c r="D17" s="37" t="n">
+        <v>100</v>
+      </c>
+      <c r="E17" s="37" t="n">
+        <f aca="false">D17/C17</f>
+        <v>2780.15961307362</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="n">
+        <v>3000</v>
+      </c>
+      <c r="C18" s="36" t="n">
+        <f aca="false"> 10^(-0.87478367-0.00043512*B18)*3.3</f>
+        <v>0.0217956723128202</v>
+      </c>
+      <c r="D18" s="37" t="n">
+        <v>100</v>
+      </c>
+      <c r="E18" s="37" t="n">
+        <f aca="false">D18/C18</f>
+        <v>4588.06677604436</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="n">
+        <v>3500</v>
+      </c>
+      <c r="C19" s="36" t="n">
+        <f aca="false"> 10^(-0.87478367-0.00043512*B19)*3.3</f>
+        <v>0.0132071852616174</v>
+      </c>
+      <c r="D19" s="37" t="n">
+        <v>100</v>
+      </c>
+      <c r="E19" s="37" t="n">
+        <f aca="false">D19/C19</f>
+        <v>7571.63604652529</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="n">
+        <v>4000</v>
+      </c>
+      <c r="C20" s="36" t="n">
+        <f aca="false"> 10^(-0.87478367-0.00043512*B20)*3.3</f>
+        <v>0.00800295306477357</v>
+      </c>
+      <c r="D20" s="37" t="n">
+        <v>100</v>
+      </c>
+      <c r="E20" s="37" t="n">
+        <f aca="false">D20/C20</f>
+        <v>12495.3875389033</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="n">
+        <v>4500</v>
+      </c>
+      <c r="C21" s="36" t="n">
+        <f aca="false"> 10^(-0.87478367-0.00043512*B21)*3.3</f>
+        <v>0.00484942525513761</v>
+      </c>
+      <c r="D21" s="37" t="n">
+        <v>100</v>
+      </c>
+      <c r="E21" s="37" t="n">
+        <f aca="false">D21/C21</f>
+        <v>20621.0003740252</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C22" s="36" t="n">
+        <f aca="false"> 10^(-0.87478367-0.00043512*B22)*3.3</f>
+        <v>0.00293853095411498</v>
+      </c>
+      <c r="D22" s="37" t="n">
+        <v>100</v>
+      </c>
+      <c r="E22" s="37" t="n">
+        <f aca="false">D22/C22</f>
+        <v>34030.609703112</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>